<commit_message>
springboot 2.7 jdk 8 base
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/templete/board.xlsx
+++ b/src/main/webapp/WEB-INF/templete/board.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev_x64\IdeaProjects\mtsSBJ3\src\main\webapp\WEB-INF\templete\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D32F392-52D6-446D-B4E5-98216AB4AFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="6360"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -35,10 +41,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${listview.brddate}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>조회수</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -49,12 +51,16 @@
   <si>
     <t>게시판</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${listview.regdate}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -144,20 +150,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -431,23 +436,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="49.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
@@ -455,7 +460,7 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -472,7 +477,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="13.5" x14ac:dyDescent="0.2">
@@ -483,10 +488,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>